<commit_message>
added parse to excel method
</commit_message>
<xml_diff>
--- a/Platform.Utilities/Templates/ContactTemplate.xlsx
+++ b/Platform.Utilities/Templates/ContactTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALFA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Platform\Platform.Utilities\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -32,15 +32,9 @@
     <t>Phone number</t>
   </si>
   <si>
-    <t>Car number</t>
-  </si>
-  <si>
     <t>Contact Type</t>
   </si>
   <si>
-    <t>Company</t>
-  </si>
-  <si>
     <t>Title (mr,mrs)</t>
   </si>
   <si>
@@ -63,16 +57,51 @@
   </si>
   <si>
     <t>VAT number</t>
+  </si>
+  <si>
+    <t>test name</t>
+  </si>
+  <si>
+    <t>ewe</t>
+  </si>
+  <si>
+    <t>mr</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>qwerty</t>
+  </si>
+  <si>
+    <t>qwe</t>
+  </si>
+  <si>
+    <t>wew@mail.com</t>
+  </si>
+  <si>
+    <t>Is Company</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,13 +124,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,73 +446,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>3809123123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>31000</v>
+      </c>
+      <c r="I2">
+        <v>232</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
         <v>12</v>
+      </c>
+      <c r="L2">
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>